<commit_message>
Uradjen backend za registraciju i prijavu
Uradjen backend za registraciju i prijavu,
dodata admin komponenta i skoro zavrsena (azuriraj metoda nije), uradjeno stilizovanje prijava strane
</commit_message>
<xml_diff>
--- a/skicaDB.xlsx
+++ b/skicaDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kosov\OneDrive\Dokumenti\UredjivanjeProstoraAPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44BD64F-8149-495A-9CF5-EB65B9A861FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D949104-1DC2-4455-B76A-7D6FA9425639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{06925BAA-4BE9-415F-B33F-E709DB16DDD4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>korisnik</t>
   </si>
@@ -176,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -191,9 +191,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -513,7 +510,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C12" sqref="C12:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +546,7 @@
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -573,14 +570,14 @@
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1</v>
@@ -597,14 +594,14 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>17</v>
@@ -621,12 +618,14 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -641,12 +640,12 @@
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -661,12 +660,12 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -681,12 +680,10 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -701,12 +698,10 @@
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -721,10 +716,10 @@
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -739,10 +734,10 @@
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -759,9 +754,7 @@
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -777,9 +770,7 @@
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>

</xml_diff>

<commit_message>
Uradjena provera pri registraciji
Odradjena provera validnosti svih polja pri registraciji (sem provere da li je mejl jedinstven)
</commit_message>
<xml_diff>
--- a/skicaDB.xlsx
+++ b/skicaDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kosov\OneDrive\Dokumenti\UredjivanjeProstoraAPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D949104-1DC2-4455-B76A-7D6FA9425639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF69D15D-5522-4DFD-987F-BDF647620065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{06925BAA-4BE9-415F-B33F-E709DB16DDD4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>korisnik</t>
   </si>
@@ -96,6 +96,30 @@
   </si>
   <si>
     <t>maticniBroj</t>
+  </si>
+  <si>
+    <t>objekat</t>
+  </si>
+  <si>
+    <t>idO</t>
+  </si>
+  <si>
+    <t>adresa</t>
+  </si>
+  <si>
+    <t>brProstorija</t>
+  </si>
+  <si>
+    <t>kvadratura</t>
+  </si>
+  <si>
+    <t>radnik</t>
+  </si>
+  <si>
+    <t>specijalizacija</t>
+  </si>
+  <si>
+    <t>brojRadnika</t>
   </si>
 </sst>
 </file>
@@ -117,7 +141,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,6 +169,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF33CC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -176,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -193,12 +229,23 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF33CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -509,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96583930-ED4F-42ED-9267-2C79E82551C8}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,6 +566,8 @@
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -534,8 +583,12 @@
       <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="E1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -558,8 +611,12 @@
       <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -582,8 +639,12 @@
       <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -606,8 +667,12 @@
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -628,8 +693,12 @@
         <v>14</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -648,8 +717,12 @@
         <v>9</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -754,7 +827,9 @@
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>

</xml_diff>

<commit_message>
Dodat rad sa objektima
Dodati modeli za objekat, rad sa bazom objekata, zapocet rad sa canvasom
</commit_message>
<xml_diff>
--- a/skicaDB.xlsx
+++ b/skicaDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kosov\OneDrive\Dokumenti\UredjivanjeProstoraAPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF69D15D-5522-4DFD-987F-BDF647620065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BF795B-CFE4-4EFF-AAC1-D1A069089BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{06925BAA-4BE9-415F-B33F-E709DB16DDD4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>korisnik</t>
   </si>
@@ -101,9 +101,6 @@
     <t>objekat</t>
   </si>
   <si>
-    <t>idO</t>
-  </si>
-  <si>
     <t>adresa</t>
   </si>
   <si>
@@ -120,6 +117,21 @@
   </si>
   <si>
     <t>brojRadnika</t>
+  </si>
+  <si>
+    <t>idR</t>
+  </si>
+  <si>
+    <t>Array[Objekat]</t>
+  </si>
+  <si>
+    <t>idSkica</t>
+  </si>
+  <si>
+    <t>_id</t>
+  </si>
+  <si>
+    <t>vlasnik</t>
   </si>
 </sst>
 </file>
@@ -557,13 +569,13 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
@@ -587,7 +599,7 @@
         <v>20</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -612,10 +624,10 @@
         <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -640,10 +652,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -668,10 +680,10 @@
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -694,10 +706,10 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -718,10 +730,10 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -741,8 +753,12 @@
         <v>10</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -754,12 +770,16 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -828,7 +848,7 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>

</xml_diff>

<commit_message>
Azuriran admin, agencije i klijenti..
Agencija sada moze da salje zahteve adminu za prosirenje broja radnih mesta i admin moze da ih razmatra. Klijent moze da salje agenciji zahtev za saradnju i agencija moze da ga razmatra
</commit_message>
<xml_diff>
--- a/skicaDB.xlsx
+++ b/skicaDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kosov\OneDrive\Dokumenti\UredjivanjeProstoraAPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F664379-606E-4393-A046-D23C5B839A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B734618-E584-48CE-BD6A-4E9C1E9D61CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{06925BAA-4BE9-415F-B33F-E709DB16DDD4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>korisnik</t>
   </si>
@@ -116,9 +116,6 @@
     <t>specijalizacija</t>
   </si>
   <si>
-    <t>brojRadnika</t>
-  </si>
-  <si>
     <t>idSkica</t>
   </si>
   <si>
@@ -165,6 +162,15 @@
   </si>
   <si>
     <t>zauzet</t>
+  </si>
+  <si>
+    <t>kapacitetRadnika</t>
+  </si>
+  <si>
+    <t>ponuda</t>
+  </si>
+  <si>
+    <t>zahtev</t>
   </si>
 </sst>
 </file>
@@ -635,14 +641,14 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" customWidth="1"/>
@@ -671,13 +677,13 @@
         <v>24</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -699,19 +705,19 @@
         <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -733,19 +739,19 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -773,7 +779,7 @@
         <v>7</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>8</v>
@@ -805,13 +811,13 @@
         <v>4</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -836,7 +842,7 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>18</v>
@@ -865,7 +871,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -881,7 +887,7 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>8</v>
@@ -889,7 +895,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -906,11 +912,13 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -957,7 +965,7 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -974,7 +982,9 @@
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>

</xml_diff>

<commit_message>
Dodat rad sa otkazivanjem posla
Klijent sada moze da posalje zahtev za otkazivanjem posla, admin taj zahtev razmatra. Ubaceno otpremanje objekta preko JSON fajla
</commit_message>
<xml_diff>
--- a/skicaDB.xlsx
+++ b/skicaDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kosov\OneDrive\Dokumenti\UredjivanjeProstoraAPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FCA03F-577F-48C5-9E9C-AECB64F8F196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BF5B8A-8079-4F87-9974-EEB82FF0A72A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{06925BAA-4BE9-415F-B33F-E709DB16DDD4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
   <si>
     <t>korisnik</t>
   </si>
@@ -171,6 +171,12 @@
   </si>
   <si>
     <t>idPosao</t>
+  </si>
+  <si>
+    <t>otkazivanjePosla</t>
+  </si>
+  <si>
+    <t>razlog</t>
   </si>
 </sst>
 </file>
@@ -192,7 +198,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,6 +256,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -313,6 +325,9 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -321,6 +336,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF99CCFF"/>
       <color rgb="FFFF7C80"/>
       <color rgb="FFCC66FF"/>
       <color rgb="FF99FF99"/>
@@ -640,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96583930-ED4F-42ED-9267-2C79E82551C8}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,6 +671,7 @@
     <col min="7" max="7" width="20.140625" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
     <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -685,7 +702,9 @@
       <c r="I1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="1"/>
+      <c r="J1" s="11" t="s">
+        <v>45</v>
+      </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -719,7 +738,9 @@
       <c r="I2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -753,7 +774,9 @@
       <c r="I3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -787,7 +810,9 @@
       <c r="I4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>

</xml_diff>

<commit_message>
Commit pre rada sa bootstrap-om
</commit_message>
<xml_diff>
--- a/skicaDB.xlsx
+++ b/skicaDB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kosov\OneDrive\Dokumenti\UredjivanjeProstoraAPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BF5B8A-8079-4F87-9974-EEB82FF0A72A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74D4511-22D4-4F5D-8745-492C6019031D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{06925BAA-4BE9-415F-B33F-E709DB16DDD4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>korisnik</t>
   </si>
@@ -177,6 +177,18 @@
   </si>
   <si>
     <t>razlog</t>
+  </si>
+  <si>
+    <t>blokiranaAgencija</t>
+  </si>
+  <si>
+    <t>datumOdblokiranja</t>
+  </si>
+  <si>
+    <t>brojPozitivnihOcena</t>
+  </si>
+  <si>
+    <t>brojOtkazanih</t>
   </si>
 </sst>
 </file>
@@ -198,7 +210,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,6 +274,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF99CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99CC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -328,6 +346,9 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,6 +357,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF99CC"/>
       <color rgb="FF99CCFF"/>
       <color rgb="FFFF7C80"/>
       <color rgb="FFCC66FF"/>
@@ -656,22 +678,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96583930-ED4F-42ED-9267-2C79E82551C8}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -705,7 +728,9 @@
       <c r="J1" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -741,7 +766,9 @@
       <c r="J2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="1"/>
+      <c r="K2" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -777,7 +804,9 @@
       <c r="J3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="1"/>
+      <c r="K3" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -813,7 +842,9 @@
       <c r="J4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="1"/>
+      <c r="K4" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -1025,7 +1056,9 @@
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>

</xml_diff>